<commit_message>
se agregan cursos dinamicos
</commit_message>
<xml_diff>
--- a/documentos/Listado de colegio.xlsx
+++ b/documentos/Listado de colegio.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\4.TESIS DE TITULO\GITCOLE\Documentos cole\documentos-6069Colegio\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Reibin\Trabajos\Tesis-Colegio\tesis-colegio\documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2425614B-58B2-4E79-B5DF-68345471DD65}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6750" activeTab="1"/>
+    <workbookView xWindow="17805" yWindow="7350" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LISTADO DE PROFESOR X CURSO" sheetId="1" r:id="rId1"/>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="962" uniqueCount="454">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="975" uniqueCount="467">
   <si>
     <t>DOCENTES</t>
   </si>
@@ -1390,12 +1391,51 @@
   </si>
   <si>
     <t>Lucero Carrión Gonzales</t>
+  </si>
+  <si>
+    <t>CM045</t>
+  </si>
+  <si>
+    <t>CM046</t>
+  </si>
+  <si>
+    <t>CM047</t>
+  </si>
+  <si>
+    <t>CM048</t>
+  </si>
+  <si>
+    <t>CM049</t>
+  </si>
+  <si>
+    <t>CM050</t>
+  </si>
+  <si>
+    <t>CM051</t>
+  </si>
+  <si>
+    <t>CM052</t>
+  </si>
+  <si>
+    <t>CM053</t>
+  </si>
+  <si>
+    <t>CM054</t>
+  </si>
+  <si>
+    <t>CM055</t>
+  </si>
+  <si>
+    <t>CM056</t>
+  </si>
+  <si>
+    <t>CM057</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1505,7 +1545,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1533,14 +1573,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1821,11 +1864,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C2:G16"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4:D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1837,26 +1880,26 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="12" t="s">
         <v>447</v>
       </c>
-      <c r="D2" s="12"/>
-      <c r="F2" s="11" t="s">
+      <c r="D2" s="13"/>
+      <c r="F2" s="12" t="s">
         <v>448</v>
       </c>
-      <c r="G2" s="12"/>
+      <c r="G2" s="13"/>
     </row>
     <row r="3" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="F3" s="13" t="s">
+      <c r="D3" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="G3" s="13" t="s">
+      <c r="G3" s="11" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1867,6 +1910,9 @@
       <c r="D4" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="E4" s="14" t="s">
+        <v>454</v>
+      </c>
       <c r="F4" s="1" t="s">
         <v>449</v>
       </c>
@@ -1881,6 +1927,9 @@
       <c r="D5" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="E5" s="14" t="s">
+        <v>455</v>
+      </c>
       <c r="F5" s="1" t="s">
         <v>16</v>
       </c>
@@ -1895,6 +1944,9 @@
       <c r="D6" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="E6" s="14" t="s">
+        <v>456</v>
+      </c>
       <c r="F6" s="1" t="s">
         <v>451</v>
       </c>
@@ -1909,6 +1961,9 @@
       <c r="D7" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="E7" s="14" t="s">
+        <v>457</v>
+      </c>
       <c r="F7" s="1" t="s">
         <v>21</v>
       </c>
@@ -1923,6 +1978,9 @@
       <c r="D8" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="E8" s="14" t="s">
+        <v>458</v>
+      </c>
       <c r="F8" s="1" t="s">
         <v>452</v>
       </c>
@@ -1937,6 +1995,9 @@
       <c r="D9" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="E9" s="14" t="s">
+        <v>459</v>
+      </c>
       <c r="F9" s="1" t="s">
         <v>17</v>
       </c>
@@ -1951,6 +2012,9 @@
       <c r="D10" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="E10" s="14" t="s">
+        <v>460</v>
+      </c>
       <c r="F10" s="1" t="s">
         <v>15</v>
       </c>
@@ -1965,6 +2029,9 @@
       <c r="D11" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="E11" s="14" t="s">
+        <v>461</v>
+      </c>
       <c r="F11" s="1" t="s">
         <v>19</v>
       </c>
@@ -1979,6 +2046,9 @@
       <c r="D12" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="E12" s="14" t="s">
+        <v>462</v>
+      </c>
       <c r="F12" s="1" t="s">
         <v>453</v>
       </c>
@@ -1993,6 +2063,9 @@
       <c r="D13" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="E13" s="14" t="s">
+        <v>463</v>
+      </c>
       <c r="F13" s="1" t="s">
         <v>23</v>
       </c>
@@ -2007,6 +2080,9 @@
       <c r="D14" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="E14" s="14" t="s">
+        <v>464</v>
+      </c>
       <c r="F14" s="1" t="s">
         <v>20</v>
       </c>
@@ -2021,6 +2097,9 @@
       <c r="D15" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="E15" s="14" t="s">
+        <v>465</v>
+      </c>
       <c r="F15" s="1" t="s">
         <v>450</v>
       </c>
@@ -2034,6 +2113,9 @@
       </c>
       <c r="D16" s="2" t="s">
         <v>25</v>
+      </c>
+      <c r="E16" s="14" t="s">
+        <v>466</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>26</v>
@@ -2052,11 +2134,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A5:D455"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7480,9 +7562,9 @@
       <c r="D455" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="A5:D455"/>
+  <autoFilter ref="A5:D455" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <hyperlinks>
-    <hyperlink ref="C61" r:id="rId1" display="http://10.102.0.225:81/user.aspx?username=cevanan&amp;userdomain=ingemmet"/>
+    <hyperlink ref="C61" r:id="rId1" display="http://10.102.0.225:81/user.aspx?username=cevanan&amp;userdomain=ingemmet" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>

<commit_message>
se sube servicio que adjunta documentos, elimina y descarga
</commit_message>
<xml_diff>
--- a/documentos/Listado de colegio.xlsx
+++ b/documentos/Listado de colegio.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Reibin\Trabajos\Tesis-Colegio\tesis-colegio\documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDF2763B-DDFF-480B-BBDE-379FEF8E6AEF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B219977E-BA59-440A-940F-BD08BD4D8D34}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8850" yWindow="1200" windowWidth="21600" windowHeight="11385" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LISTADO DE PROFESOR X CURSO" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6380" uniqueCount="2153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6347" uniqueCount="2148">
   <si>
     <t>DOCENTES</t>
   </si>
@@ -6440,27 +6440,6 @@
     <t>AL-CL2020-000019</t>
   </si>
   <si>
-    <t>AL-CL2020-000020</t>
-  </si>
-  <si>
-    <t>AL-CL2020-000021</t>
-  </si>
-  <si>
-    <t>AL-CL2020-000022</t>
-  </si>
-  <si>
-    <t>AL-CL2020-000023</t>
-  </si>
-  <si>
-    <t>AL-CL2020-000024</t>
-  </si>
-  <si>
-    <t>AL-CL2020-000025</t>
-  </si>
-  <si>
-    <t>AL-CL2020-000026</t>
-  </si>
-  <si>
     <t>INSERT tbl_ClaseAlumno(codigo,codigoAlumno,codigoClase) values(</t>
   </si>
   <si>
@@ -6504,6 +6483,12 @@
   </si>
   <si>
     <t>values('MAT2020-12-00001','CL2020-00001','AL2020-00001_PRESENTACION_01.docx',8,'2020')</t>
+  </si>
+  <si>
+    <t xml:space="preserve">insert into </t>
+  </si>
+  <si>
+    <t xml:space="preserve">insert tbl_material (codigo, codigoClase, semana, periodo, usuario,nombreMaterial,tarea,fechaInicio,fechaFin) </t>
   </si>
 </sst>
 </file>
@@ -7800,7 +7785,7 @@
   <dimension ref="B2:K126"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:B118"/>
+      <selection activeCell="F132" sqref="F132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -41430,10 +41415,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3484CF4A-8D35-4379-AAC1-A72AA47DBAC8}">
-  <dimension ref="C1:G9"/>
+  <dimension ref="C1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -41442,15 +41427,15 @@
     <col min="4" max="4" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C1" s="29" t="s">
-        <v>2140</v>
+        <v>2133</v>
       </c>
       <c r="D1" s="29"/>
       <c r="E1" s="29"/>
       <c r="F1" s="29"/>
     </row>
-    <row r="2" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
         <v>451</v>
       </c>
@@ -41458,18 +41443,18 @@
         <v>450</v>
       </c>
       <c r="E2" t="s">
-        <v>2139</v>
+        <v>2132</v>
       </c>
       <c r="F2" t="s">
         <v>455</v>
       </c>
       <c r="G2" t="s">
-        <v>2148</v>
-      </c>
-    </row>
-    <row r="3" spans="3:7" x14ac:dyDescent="0.25">
+        <v>2141</v>
+      </c>
+    </row>
+    <row r="3" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
-        <v>2141</v>
+        <v>2134</v>
       </c>
       <c r="D3" s="23" t="s">
         <v>516</v>
@@ -41481,12 +41466,15 @@
         <v>2020</v>
       </c>
       <c r="G3" t="s">
-        <v>2149</v>
-      </c>
-    </row>
-    <row r="4" spans="3:7" x14ac:dyDescent="0.25">
+        <v>2142</v>
+      </c>
+      <c r="H3" t="s">
+        <v>2146</v>
+      </c>
+    </row>
+    <row r="4" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
-        <v>2142</v>
+        <v>2135</v>
       </c>
       <c r="D4" s="23" t="s">
         <v>516</v>
@@ -41498,12 +41486,12 @@
         <v>2020</v>
       </c>
       <c r="G4" t="s">
-        <v>2149</v>
-      </c>
-    </row>
-    <row r="5" spans="3:7" x14ac:dyDescent="0.25">
+        <v>2142</v>
+      </c>
+    </row>
+    <row r="5" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
-        <v>2143</v>
+        <v>2136</v>
       </c>
       <c r="D5" s="23" t="s">
         <v>516</v>
@@ -41515,12 +41503,12 @@
         <v>2020</v>
       </c>
       <c r="G5" t="s">
-        <v>2149</v>
-      </c>
-    </row>
-    <row r="6" spans="3:7" x14ac:dyDescent="0.25">
+        <v>2142</v>
+      </c>
+    </row>
+    <row r="6" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
-        <v>2144</v>
+        <v>2137</v>
       </c>
       <c r="D6" s="23" t="s">
         <v>516</v>
@@ -41532,12 +41520,12 @@
         <v>2020</v>
       </c>
       <c r="G6" t="s">
-        <v>2149</v>
-      </c>
-    </row>
-    <row r="7" spans="3:7" x14ac:dyDescent="0.25">
+        <v>2142</v>
+      </c>
+    </row>
+    <row r="7" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
-        <v>2145</v>
+        <v>2138</v>
       </c>
       <c r="D7" s="23" t="s">
         <v>516</v>
@@ -41549,12 +41537,12 @@
         <v>2020</v>
       </c>
       <c r="G7" t="s">
-        <v>2149</v>
-      </c>
-    </row>
-    <row r="8" spans="3:7" x14ac:dyDescent="0.25">
+        <v>2142</v>
+      </c>
+    </row>
+    <row r="8" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
-        <v>2146</v>
+        <v>2139</v>
       </c>
       <c r="D8" s="23" t="s">
         <v>516</v>
@@ -41566,12 +41554,12 @@
         <v>2020</v>
       </c>
       <c r="G8" t="s">
-        <v>2149</v>
-      </c>
-    </row>
-    <row r="9" spans="3:7" x14ac:dyDescent="0.25">
+        <v>2142</v>
+      </c>
+    </row>
+    <row r="9" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
-        <v>2147</v>
+        <v>2140</v>
       </c>
       <c r="D9" s="23" t="s">
         <v>516</v>
@@ -41583,7 +41571,12 @@
         <v>2020</v>
       </c>
       <c r="G9" t="s">
-        <v>2149</v>
+        <v>2142</v>
+      </c>
+    </row>
+    <row r="12" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>2147</v>
       </c>
     </row>
   </sheetData>
@@ -41600,8 +41593,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1F3FD73-A620-44C6-B360-8C2D8BABD914}">
   <dimension ref="B1:G27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2:G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -41635,7 +41628,7 @@
         <v>1013</v>
       </c>
       <c r="F2" t="s">
-        <v>2138</v>
+        <v>2131</v>
       </c>
       <c r="G2" t="str">
         <f>_xlfn.CONCAT(F2,E2,B2,E2,",",E2,C2,E2,",",E2,D2,E2,");")</f>
@@ -41656,10 +41649,10 @@
         <v>1013</v>
       </c>
       <c r="F3" t="s">
-        <v>2138</v>
+        <v>2131</v>
       </c>
       <c r="G3" t="str">
-        <f t="shared" ref="G3:G27" si="0">_xlfn.CONCAT(F3,E3,B3,E3,",",E3,C3,E3,",",E3,D3,E3,");")</f>
+        <f t="shared" ref="G3:G20" si="0">_xlfn.CONCAT(F3,E3,B3,E3,",",E3,C3,E3,",",E3,D3,E3,");")</f>
         <v>INSERT tbl_ClaseAlumno(codigo,codigoAlumno,codigoClase) values("AL-CL2020-000002","AL2020-00001","CL2020-00010");</v>
       </c>
     </row>
@@ -41677,7 +41670,7 @@
         <v>1013</v>
       </c>
       <c r="F4" t="s">
-        <v>2138</v>
+        <v>2131</v>
       </c>
       <c r="G4" t="str">
         <f t="shared" si="0"/>
@@ -41698,7 +41691,7 @@
         <v>1013</v>
       </c>
       <c r="F5" t="s">
-        <v>2138</v>
+        <v>2131</v>
       </c>
       <c r="G5" t="str">
         <f t="shared" si="0"/>
@@ -41719,7 +41712,7 @@
         <v>1013</v>
       </c>
       <c r="F6" t="s">
-        <v>2138</v>
+        <v>2131</v>
       </c>
       <c r="G6" t="str">
         <f t="shared" si="0"/>
@@ -41740,7 +41733,7 @@
         <v>1013</v>
       </c>
       <c r="F7" t="s">
-        <v>2138</v>
+        <v>2131</v>
       </c>
       <c r="G7" t="str">
         <f t="shared" si="0"/>
@@ -41761,7 +41754,7 @@
         <v>1013</v>
       </c>
       <c r="F8" t="s">
-        <v>2138</v>
+        <v>2131</v>
       </c>
       <c r="G8" t="str">
         <f t="shared" si="0"/>
@@ -41782,7 +41775,7 @@
         <v>1013</v>
       </c>
       <c r="F9" t="s">
-        <v>2138</v>
+        <v>2131</v>
       </c>
       <c r="G9" t="str">
         <f t="shared" si="0"/>
@@ -41803,7 +41796,7 @@
         <v>1013</v>
       </c>
       <c r="F10" t="s">
-        <v>2138</v>
+        <v>2131</v>
       </c>
       <c r="G10" t="str">
         <f t="shared" si="0"/>
@@ -41824,7 +41817,7 @@
         <v>1013</v>
       </c>
       <c r="F11" t="s">
-        <v>2138</v>
+        <v>2131</v>
       </c>
       <c r="G11" t="str">
         <f t="shared" si="0"/>
@@ -41845,7 +41838,7 @@
         <v>1013</v>
       </c>
       <c r="F12" t="s">
-        <v>2138</v>
+        <v>2131</v>
       </c>
       <c r="G12" t="str">
         <f t="shared" si="0"/>
@@ -41866,7 +41859,7 @@
         <v>1013</v>
       </c>
       <c r="F13" t="s">
-        <v>2138</v>
+        <v>2131</v>
       </c>
       <c r="G13" t="str">
         <f t="shared" si="0"/>
@@ -41887,7 +41880,7 @@
         <v>1013</v>
       </c>
       <c r="F14" t="s">
-        <v>2138</v>
+        <v>2131</v>
       </c>
       <c r="G14" t="str">
         <f t="shared" si="0"/>
@@ -41908,7 +41901,7 @@
         <v>1013</v>
       </c>
       <c r="F15" t="s">
-        <v>2138</v>
+        <v>2131</v>
       </c>
       <c r="G15" t="str">
         <f t="shared" si="0"/>
@@ -41929,7 +41922,7 @@
         <v>1013</v>
       </c>
       <c r="F16" t="s">
-        <v>2138</v>
+        <v>2131</v>
       </c>
       <c r="G16" t="str">
         <f t="shared" si="0"/>
@@ -41950,7 +41943,7 @@
         <v>1013</v>
       </c>
       <c r="F17" t="s">
-        <v>2138</v>
+        <v>2131</v>
       </c>
       <c r="G17" t="str">
         <f t="shared" si="0"/>
@@ -41971,7 +41964,7 @@
         <v>1013</v>
       </c>
       <c r="F18" t="s">
-        <v>2138</v>
+        <v>2131</v>
       </c>
       <c r="G18" t="str">
         <f t="shared" si="0"/>
@@ -41992,7 +41985,7 @@
         <v>1013</v>
       </c>
       <c r="F19" t="s">
-        <v>2138</v>
+        <v>2131</v>
       </c>
       <c r="G19" t="str">
         <f t="shared" si="0"/>
@@ -42013,7 +42006,7 @@
         <v>1013</v>
       </c>
       <c r="F20" t="s">
-        <v>2138</v>
+        <v>2131</v>
       </c>
       <c r="G20" t="str">
         <f t="shared" si="0"/>
@@ -42021,151 +42014,39 @@
       </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
-        <v>2131</v>
-      </c>
-      <c r="C21" s="17" t="s">
-        <v>550</v>
-      </c>
-      <c r="D21" s="17" t="s">
-        <v>1009</v>
-      </c>
-      <c r="E21" s="22" t="s">
-        <v>1013</v>
-      </c>
-      <c r="F21" t="s">
-        <v>2138</v>
-      </c>
-      <c r="G21" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT tbl_ClaseAlumno(codigo,codigoAlumno,codigoClase) values("AL-CL2020-000020","AL2020-00002","CL2020-00043");</v>
-      </c>
+      <c r="C21" s="17"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="22"/>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
-        <v>2132</v>
-      </c>
-      <c r="C22" s="17" t="s">
-        <v>550</v>
-      </c>
-      <c r="D22" s="17" t="s">
-        <v>1000</v>
-      </c>
-      <c r="E22" s="22" t="s">
-        <v>1013</v>
-      </c>
-      <c r="F22" t="s">
-        <v>2138</v>
-      </c>
-      <c r="G22" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT tbl_ClaseAlumno(codigo,codigoAlumno,codigoClase) values("AL-CL2020-000021","AL2020-00002","CL2020-00034");</v>
-      </c>
+      <c r="C22" s="17"/>
+      <c r="D22" s="17"/>
+      <c r="E22" s="22"/>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
-        <v>2133</v>
-      </c>
-      <c r="C23" s="17" t="s">
-        <v>550</v>
-      </c>
-      <c r="D23" s="17" t="s">
-        <v>1009</v>
-      </c>
-      <c r="E23" s="22" t="s">
-        <v>1013</v>
-      </c>
-      <c r="F23" t="s">
-        <v>2138</v>
-      </c>
-      <c r="G23" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT tbl_ClaseAlumno(codigo,codigoAlumno,codigoClase) values("AL-CL2020-000022","AL2020-00002","CL2020-00043");</v>
-      </c>
+      <c r="C23" s="17"/>
+      <c r="D23" s="17"/>
+      <c r="E23" s="22"/>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
-        <v>2134</v>
-      </c>
-      <c r="C24" s="17" t="s">
-        <v>550</v>
-      </c>
-      <c r="D24" s="17" t="s">
-        <v>1000</v>
-      </c>
-      <c r="E24" s="22" t="s">
-        <v>1013</v>
-      </c>
-      <c r="F24" t="s">
-        <v>2138</v>
-      </c>
-      <c r="G24" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT tbl_ClaseAlumno(codigo,codigoAlumno,codigoClase) values("AL-CL2020-000023","AL2020-00002","CL2020-00034");</v>
-      </c>
+      <c r="C24" s="17"/>
+      <c r="D24" s="17"/>
+      <c r="E24" s="22"/>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
-        <v>2135</v>
-      </c>
-      <c r="C25" s="17" t="s">
-        <v>550</v>
-      </c>
-      <c r="D25" s="17" t="s">
-        <v>1009</v>
-      </c>
-      <c r="E25" s="22" t="s">
-        <v>1013</v>
-      </c>
-      <c r="F25" t="s">
-        <v>2138</v>
-      </c>
-      <c r="G25" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT tbl_ClaseAlumno(codigo,codigoAlumno,codigoClase) values("AL-CL2020-000024","AL2020-00002","CL2020-00043");</v>
-      </c>
+      <c r="C25" s="17"/>
+      <c r="D25" s="17"/>
+      <c r="E25" s="22"/>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
-        <v>2136</v>
-      </c>
-      <c r="C26" s="17" t="s">
-        <v>550</v>
-      </c>
-      <c r="D26" s="17" t="s">
-        <v>1000</v>
-      </c>
-      <c r="E26" s="22" t="s">
-        <v>1013</v>
-      </c>
-      <c r="F26" t="s">
-        <v>2138</v>
-      </c>
-      <c r="G26" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT tbl_ClaseAlumno(codigo,codigoAlumno,codigoClase) values("AL-CL2020-000025","AL2020-00002","CL2020-00034");</v>
-      </c>
+      <c r="C26" s="17"/>
+      <c r="D26" s="17"/>
+      <c r="E26" s="22"/>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B27" t="s">
-        <v>2137</v>
-      </c>
-      <c r="C27" s="17" t="s">
-        <v>550</v>
-      </c>
-      <c r="D27" s="17" t="s">
-        <v>1009</v>
-      </c>
-      <c r="E27" s="22" t="s">
-        <v>1013</v>
-      </c>
-      <c r="F27" t="s">
-        <v>2138</v>
-      </c>
-      <c r="G27" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT tbl_ClaseAlumno(codigo,codigoAlumno,codigoClase) values("AL-CL2020-000026","AL2020-00002","CL2020-00043");</v>
-      </c>
+      <c r="C27" s="17"/>
+      <c r="D27" s="17"/>
+      <c r="E27" s="22"/>
     </row>
   </sheetData>
   <autoFilter ref="B1:G27" xr:uid="{51F6D30C-6281-4EF0-A794-10F06B856BD1}"/>
@@ -42178,7 +42059,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC2D1812-9805-4BDC-AEC2-F589169DEE71}">
   <dimension ref="D5:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
@@ -42189,17 +42070,17 @@
   <sheetData>
     <row r="5" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D5" t="s">
-        <v>2150</v>
+        <v>2143</v>
       </c>
     </row>
     <row r="6" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D6" t="s">
-        <v>2151</v>
+        <v>2144</v>
       </c>
     </row>
     <row r="7" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D7" t="s">
-        <v>2152</v>
+        <v>2145</v>
       </c>
     </row>
   </sheetData>

</xml_diff>